<commit_message>
Modification de dernière minutes sur les docs
Signed-off-by: Benjamin BRAYE <benjamin.braye@viacesi.fr>
</commit_message>
<xml_diff>
--- a/Documentation/Livrables/planning pour présentation.xlsx
+++ b/Documentation/Livrables/planning pour présentation.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benjamin BRAYE\Desktop\j-sim-forest\Documentation\Livrables\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="23715" windowHeight="10545"/>
   </bookViews>
@@ -55,7 +60,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,8 +76,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -82,12 +108,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -137,23 +157,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -163,6 +184,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -211,7 +235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,7 +270,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,7 +482,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection sqref="A1:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,36 +492,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4">
+      <c r="C1" s="9">
         <v>41306</v>
       </c>
-      <c r="D1" s="4">
+      <c r="D1" s="9">
         <v>41309</v>
       </c>
-      <c r="E1" s="4">
+      <c r="E1" s="9">
         <v>41310</v>
       </c>
-      <c r="F1" s="4">
+      <c r="F1" s="9">
         <v>41311</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="9">
         <v>41312</v>
       </c>
-      <c r="H1" s="4">
+      <c r="H1" s="9">
         <v>41313</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="2"/>
@@ -508,8 +532,8 @@
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="10"/>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="2"/>
@@ -520,8 +544,8 @@
       <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" s="8" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="2"/>
@@ -532,8 +556,8 @@
       <c r="H4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="2"/>
@@ -544,11 +568,11 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2"/>
@@ -558,9 +582,9 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="2"/>
@@ -570,11 +594,11 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="2"/>
@@ -584,32 +608,32 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="G9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="A10" s="10"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="2"/>
@@ -618,47 +642,47 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
+      <c r="A11" s="10"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
+      <c r="A12" s="10"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D13" s="2"/>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F13" s="2"/>
@@ -666,46 +690,46 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
+      <c r="A14" s="10"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="8" t="s">
+      <c r="E14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H14" s="8" t="s">
+      <c r="H14" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="9" t="s">
+      <c r="B15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>9</v>
       </c>
     </row>
@@ -717,7 +741,7 @@
     <mergeCell ref="A13:A14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>